<commit_message>
# some manipulations made with the data as a dictionary
</commit_message>
<xml_diff>
--- a/exercise_1/linear_regression_df.xlsx
+++ b/exercise_1/linear_regression_df.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17668"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E277460\PycharmProjects\Jupyter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Python\pandas\exercise_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8592"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8595"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" calcOnSave="0"/>
+  <calcPr calcId="152511" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>X</t>
   </si>
@@ -44,13 +44,16 @@
     <t>119.4</t>
   </si>
   <si>
-    <t>15.7</t>
+    <t>200</t>
+  </si>
+  <si>
+    <t>z</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -398,23 +401,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D2" sqref="D2:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -424,8 +430,11 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -435,8 +444,11 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -446,8 +458,11 @@
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -457,8 +472,11 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -467,6 +485,51 @@
       </c>
       <c r="C6" t="s">
         <v>5</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>55</v>
+      </c>
+      <c r="C7">
+        <v>88</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>70</v>
+      </c>
+      <c r="C8">
+        <v>300</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="C9">
+        <v>400</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>